<commit_message>
Trabajando en los issues 105 a 108
GithubOrganizationEnquirer
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTest.xlsx
+++ b/src/test/resources/excelTest.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCENCIA\factoriaSoftware\Audit4Improve22-23\Audit4Improve-API\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC655F3E-7AB5-4883-B9AE-5A0605A2270F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="3675" yWindow="5415" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="entidadTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +24,89 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+  <si>
+    <t xml:space="preserve">Métricas guardadas el día </t>
+  </si>
+  <si>
+    <t>Indicadores</t>
+  </si>
+  <si>
+    <t>downloads</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>Descargas realizadas</t>
+  </si>
+  <si>
+    <t>lastPush</t>
+  </si>
+  <si>
+    <t>2-2-22</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Último push realizado en el repositorio</t>
+  </si>
+  <si>
+    <t>otracosa</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>cosas</t>
+  </si>
+  <si>
+    <t>Indicador Ejemplo</t>
+  </si>
+  <si>
+    <t>CRITICAL</t>
+  </si>
+  <si>
+    <t>indicador2</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>unidad2</t>
+  </si>
+  <si>
+    <t>Indicador Ejemplo 2</t>
+  </si>
+  <si>
+    <t>WARNING</t>
+  </si>
+  <si>
+    <t>indicador3</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>unidad3</t>
+  </si>
+  <si>
+    <t>IndicadorEjemplo3</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 18:07:36 CET 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 17:07:36 CET 2024</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +114,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF00FF00"/>
+      <name val="Serif"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Dialog"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFC800"/>
+      <name val="Serif"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFC800"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +168,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +452,129 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mejoras de GitHubOrganizationEnquirer y sus tests
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTest.xlsx
+++ b/src/test/resources/excelTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCENCIA\factoriaSoftware\Audit4Improve22-23\Audit4Improve-API\src\test\resources\"/>
     </mc:Choice>
@@ -13,11 +13,11 @@
     <workbookView xWindow="3675" yWindow="5415" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="entidadTest" sheetId="1" r:id="rId1"/>
+    <sheet name="entidadTest" r:id="rId5" sheetId="1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
   <si>
     <t xml:space="preserve">Métricas guardadas el día </t>
   </si>
@@ -100,13 +100,20 @@
   </si>
   <si>
     <t>Tue Mar 05 17:07:36 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 12:39:48 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 11:39:48 CET 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <numFmts count="0"/>
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +138,24 @@
       <sz val="10"/>
       <color rgb="FFFFC800"/>
       <name val="Serif"/>
+    </font>
+    <font>
+      <name val="Serif"/>
+      <sz val="10.0"/>
+      <color rgb="FF00FF00"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Dialog"/>
+      <sz val="12.0"/>
+      <color rgb="FFFF0000"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Serif"/>
+      <sz val="10.0"/>
+      <color rgb="FFFFC800"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="5">
@@ -168,11 +193,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,129 +480,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.9375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="24.55859375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="9.703125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="32.12109375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="24.55859375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.1328125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="24.55859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>23</v>
+      <c r="B1" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
-        <v>24</v>
+      <c r="E2" s="0"/>
+      <c r="F2" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
+    <row r="3">
+      <c r="A3" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
+      <c r="E3" s="0"/>
+      <c r="F3" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75">
-      <c r="A5" s="2" t="s">
+    <row r="5">
+      <c r="A5" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G5" t="s">
-        <v>24</v>
+      <c r="F5" s="0"/>
+      <c r="G5" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="3" t="s">
+    <row r="6">
+      <c r="A6" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
-        <v>24</v>
+      <c r="F6" s="0"/>
+      <c r="G6" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75">
-      <c r="A7" s="2" t="s">
+    <row r="7">
+      <c r="A7" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G7" t="s">
-        <v>24</v>
+      <c r="F7" s="0"/>
+      <c r="G7" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
101 a 104: Cambios en GitHubRepositoryEnquierer
Falta la métrica de commits en el último sprint
Es necesario mejorar los tests
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTest.xlsx
+++ b/src/test/resources/excelTest.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="119">
   <si>
     <t xml:space="preserve">Métricas guardadas el día </t>
   </si>
@@ -200,6 +200,189 @@
   </si>
   <si>
     <t>Fri Mar 08 14:41:12 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 14:53:52 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 14:55:48 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 14:55:47 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 13:45:32 CET 2024</t>
+  </si>
+  <si>
+    <t>totalAdditions</t>
+  </si>
+  <si>
+    <t>6909</t>
+  </si>
+  <si>
+    <t>additions</t>
+  </si>
+  <si>
+    <t>Suma el total de adiciones desde que el repositorio se creó</t>
+  </si>
+  <si>
+    <t>GitHub, calculada</t>
+  </si>
+  <si>
+    <t>totalDeletions</t>
+  </si>
+  <si>
+    <t>deletions</t>
+  </si>
+  <si>
+    <t>Suma el total de eliminaciones desde que el repositorio se cre�</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 14:56:46 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 14:56:45 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 14:56:44 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 14:59:31 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:01:05 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:01:04 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:17:30 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:17:28 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:17:59 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:21:45 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:21:44 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:22:10 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:22:09 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:22:43 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:23:03 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:23:02 CET 2024</t>
+  </si>
+  <si>
+    <t>ownerCommits</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>commits</t>
+  </si>
+  <si>
+    <t>Commits del responsable</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:23:01 CET 2024</t>
+  </si>
+  <si>
+    <t>collaborators</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>Numero de colaboradores en el repositorio</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:33:21 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:33:19 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:33:20 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:33:18 CET 2024</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>Numero de asuntos totales</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:34:41 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:34:38 CET 2024</t>
+  </si>
+  <si>
+    <t>closedIssues</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>Numero de asuntos cerrados</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:34:40 CET 2024</t>
+  </si>
+  <si>
+    <t>openIssues</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:37:03 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:37:00 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:37:02 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:36:59 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:37:34 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:37:31 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:37:33 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:37:30 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:37:32 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:38:21 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:38:18 CET 2024</t>
+  </si>
+  <si>
+    <t>Fri Mar 08 15:38:20 CET 2024</t>
   </si>
 </sst>
 </file>
@@ -207,7 +390,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="12">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +432,78 @@
       <name val="Serif"/>
       <sz val="10.0"/>
       <color rgb="FFFFC800"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Serif"/>
+      <sz val="10.0"/>
+      <color rgb="FF00FF00"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Serif"/>
+      <sz val="10.0"/>
+      <color rgb="FF00FF00"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Serif"/>
+      <sz val="10.0"/>
+      <color rgb="FF00FF00"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Serif"/>
+      <sz val="10.0"/>
+      <color rgb="FF00FF00"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Serif"/>
+      <sz val="10.0"/>
+      <color rgb="FF00FF00"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Serif"/>
+      <sz val="10.0"/>
+      <color rgb="FF00FF00"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Serif"/>
+      <sz val="10.0"/>
+      <color rgb="FF00FF00"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Serif"/>
+      <sz val="10.0"/>
+      <color rgb="FF00FF00"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Serif"/>
+      <sz val="10.0"/>
+      <color rgb="FF00FF00"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Serif"/>
+      <sz val="10.0"/>
+      <color rgb="FF00FF00"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Serif"/>
+      <sz val="10.0"/>
+      <color rgb="FF00FF00"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Serif"/>
+      <sz val="10.0"/>
+      <color rgb="FF00FF00"/>
       <b val="true"/>
     </font>
     <font>
@@ -317,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -330,6 +585,18 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,7 +1011,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -752,9 +1019,9 @@
   <cols>
     <col min="1" max="1" width="21.9375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="25.796875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="50.90625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="6.58984375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.52734375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="51.4921875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.01171875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="24.55859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -763,14 +1030,14 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>56</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="11">
+      <c r="A2" t="s" s="23">
         <v>28</v>
       </c>
-      <c r="B2" t="s" s="11">
+      <c r="B2" t="s" s="23">
         <v>29</v>
       </c>
       <c r="C2" t="s" s="0">
@@ -783,151 +1050,271 @@
         <v>31</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>57</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="11">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s" s="11">
-        <v>41</v>
+      <c r="A3" t="s" s="23">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s" s="23">
+        <v>103</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>31</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>57</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="11">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s" s="11">
-        <v>52</v>
+      <c r="A4" t="s" s="23">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s" s="23">
+        <v>87</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>31</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>57</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="11">
+      <c r="A5" t="s" s="23">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s" s="23">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="23">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s" s="23">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="23">
         <v>33</v>
       </c>
-      <c r="B5" t="s" s="11">
+      <c r="B7" t="s" s="23">
         <v>34</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C7" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D7" t="s" s="0">
         <v>35</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="11">
-        <v>36</v>
-      </c>
-      <c r="B6" t="s" s="11">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="11">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s" s="11">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>43</v>
       </c>
       <c r="E7" t="s" s="0">
         <v>31</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>57</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="11">
-        <v>44</v>
-      </c>
-      <c r="B8" t="s" s="11">
-        <v>15</v>
+      <c r="A8" t="s" s="23">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s" s="23">
+        <v>37</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s" s="0">
         <v>31</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>57</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="11">
-        <v>46</v>
-      </c>
-      <c r="B9" t="s" s="11">
-        <v>47</v>
+      <c r="A9" t="s" s="23">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s" s="23">
+        <v>37</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s" s="0">
         <v>31</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>57</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s" s="23">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s" s="23">
+        <v>98</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="23">
+        <v>106</v>
+      </c>
+      <c r="B11" t="s" s="23">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="23">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s" s="23">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="23">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s" s="23">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="23">
+        <v>91</v>
+      </c>
+      <c r="B14" t="s" s="23">
+        <v>92</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="23">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s" s="23">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
         <v>1</v>
       </c>
     </row>

</xml_diff>